<commit_message>
parallel execution and test fixes
</commit_message>
<xml_diff>
--- a/src/test/resources/Testdata/TestData.xlsx
+++ b/src/test/resources/Testdata/TestData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\AssignmentThreeWithPOM\AssignmentThreeWithPOM\src\test\resources\Testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Automation\New folder\QAAssignment3\src\test\resources\Testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{622F19E7-3995-410B-A3F0-3B199AE5BE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C962B1C-AE72-4556-A0D4-8E78517F52E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1900" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
-  <si>
-    <t>Brand</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>dress</t>
   </si>
@@ -40,17 +37,19 @@
     <t>camera</t>
   </si>
   <si>
-    <t>Samsung is the phone</t>
-  </si>
-  <si>
     <t>Samsung Selected</t>
+  </si>
+  <si>
+    <t>Watch</t>
+  </si>
+  <si>
+    <t>Jewelry &amp; Watches</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -362,38 +361,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C4"/>
+  <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B2" sqref="B2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.54296875"/>
-    <col min="2" max="2" customWidth="true" width="12.90625"/>
-    <col min="3" max="3" customWidth="true" width="26.1796875"/>
+    <col min="1" max="1" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.08984375" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s" s="0">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3" t="s" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B4" t="s" s="0">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -413,7 +415,7 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B2" s="0">
+      <c r="B2">
         <v>150000</v>
       </c>
     </row>

</xml_diff>